<commit_message>
version 2 - Multiprocessing & progress bar
</commit_message>
<xml_diff>
--- a/찹찹 길드원 현황.xlsx
+++ b/찹찹 길드원 현황.xlsx
@@ -456,49 +456,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>준대</t>
+          <t>희철</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>팬텀</t>
+          <t>팔라딘</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>49</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>희철</t>
+          <t>더엔도적</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>252</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>팔라딘</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -513,29 +513,29 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2020년  10월 11일</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>더엔도적</t>
+          <t>준대</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>팬텀</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -545,7 +545,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2020년  10월 11일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
@@ -584,54 +584,54 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>용띨</t>
+          <t>재수강</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>258</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>소울마스터</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>54</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2020년  12월 20일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>재수강</t>
+          <t>또속니친구야</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>252</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>루미너스</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>51</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -680,59 +680,59 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>또속니친구야</t>
+          <t>용띨</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>루미너스</t>
+          <t>소울마스터</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2020년  12월 20일</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>세졍</t>
+          <t>현최</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>258</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>비숍</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>54</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -776,27 +776,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>현최</t>
+          <t>진주콰외구함</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>나이트로드</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -808,17 +808,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>진주콰외구함</t>
+          <t>세졍</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>나이트로드</t>
+          <t>비숍</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -840,49 +840,49 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>얼음은각얼음</t>
+          <t>아란접을래</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>아크메이지(썬,콜)</t>
+          <t>아란</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>검사직업up</t>
+          <t>욕엉</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>256</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>엔젤릭버스터</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -892,71 +892,71 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>53</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2020년  12월 20일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>아란접을래</t>
+          <t>검사직업up</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>258</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>아란</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>53</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2020년  12월 20일</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>욕엉</t>
+          <t>얼음은각얼음</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>엔젤릭버스터</t>
+          <t>아크메이지(썬,콜)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -968,123 +968,123 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>관악구자취러</t>
+          <t>봉인된일리움</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>일리움</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>반화련</t>
+          <t>뚜안</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>257</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>비숍</t>
+          <t>스트라이커</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>51</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2020년  11월 15일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>봉인된일리움</t>
+          <t>반화련</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>257</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>일리움</t>
+          <t>비숍</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2020년  11월 15일</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>뚜안</t>
+          <t>관악구자취러</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>249</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>스트라이커</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1096,91 +1096,91 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>쿠무스</t>
+          <t>뻬줘</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>캐논마스터</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2021년  2월 24일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Aremene</t>
+          <t>경시</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>249</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>메르세데스</t>
+          <t>나이트로드</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>54</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>뻬줘</t>
+          <t>Aremene</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>254</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>캐논마스터</t>
+          <t>메르세데스</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>경시</t>
+          <t>쿠무스</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>나이트로드</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1212,71 +1212,71 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>54</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2021년  2월 24일</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>한선생</t>
+          <t>랄로님이다</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>팬텀</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>절계</t>
+          <t>지평선</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>245</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>호영</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1288,27 +1288,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>랄로님이다</t>
+          <t>절계</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>254</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>팬텀</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1320,49 +1320,49 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>지평선</t>
+          <t>한선생</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>249</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>호영</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>킁카츄</t>
+          <t>뉴둥</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>미하일</t>
+          <t>에반</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1372,167 +1372,167 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>동녘동옥돌민</t>
+          <t>신속한에반</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>241</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>은월</t>
+          <t>에반</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021년  1월 24일</t>
+          <t>2020년  12월 13일</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>뉴둥</t>
+          <t>동녘동옥돌민</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>253</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>에반</t>
+          <t>은월</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>56</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>56</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2021년  1월 24일</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>신속한에반</t>
+          <t>킁카츄</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>247</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>에반</t>
+          <t>미하일</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>48</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2020년  12월 13일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>경슥</t>
+          <t>쿵지</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>에반</t>
+          <t>아크메이지(불,독)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>51</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2020년  11월 15일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>구칠이년</t>
+          <t>오재용</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>아크메이지(불,독)</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1544,12 +1544,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>쿵지</t>
+          <t>구칠이년</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>253</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1559,433 +1559,433 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>53</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>53</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>오재용</t>
+          <t>경슥</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>247</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>에반</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2020년  11월 15일</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>롱형</t>
+          <t>토성씨</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>패스파인더</t>
+          <t>배틀메이지</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021년  2월 24일</t>
+          <t>2021년  1월 24일</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>StoneIdol</t>
+          <t>시니영</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>274</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>엔젤릭버스터</t>
+          <t>섀도어</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>59</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>54</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>토성씨</t>
+          <t>StoneIdol</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>252</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>배틀메이지</t>
+          <t>엔젤릭버스터</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021년  1월 24일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>시니영</t>
+          <t>롱형</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>274</t>
+          <t>247</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>섀도어</t>
+          <t>패스파인더</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>51</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 24일</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>흐재</t>
+          <t>눈산토끼</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>나이트로드</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2020년  11월 29일</t>
+          <t>2020년  11월 8일</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>짱난잉</t>
+          <t>EnergyBolt</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>아란</t>
+          <t>아크메이지(불,독)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>54</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>54</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021년  2월 24일</t>
+          <t>2020년  9월 6일</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>눈산토끼</t>
+          <t>짱난잉</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>252</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>나이트로드</t>
+          <t>아란</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2020년  11월 8일</t>
+          <t>2021년  2월 24일</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>EnergyBolt</t>
+          <t>흐재</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>247</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>아크메이지(불,독)</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>51</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2020년  9월 6일</t>
+          <t>2020년  11월 29일</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>기묘한대통령</t>
+          <t>셔노</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>246</t>
+          <t>250</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>루미너스</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2020년  12월 6일</t>
+          <t>2020년  9월 27일</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>쮸에몬</t>
+          <t>브리바첸</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>267</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>패스파인더</t>
+          <t>데몬어벤져</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>53</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>셔노</t>
+          <t>쮸에몬</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>252</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>루미너스</t>
+          <t>패스파인더</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2020년  9월 27일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>브리바첸</t>
+          <t>기묘한대통령</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>246</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>데몬어벤져</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2020년  12월 6일</t>
         </is>
       </c>
     </row>
@@ -2760,64 +2760,64 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>박이초</t>
+          <t>도챙</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>246</t>
+          <t>244</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>히어로</t>
+          <t>엔젤릭버스터</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>도챙</t>
+          <t>박이초</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>246</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>엔젤릭버스터</t>
+          <t>히어로</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>54</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
@@ -2888,12 +2888,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>현수기인</t>
+          <t>김콧치냥</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>244</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2903,29 +2903,29 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2021년  2월 24일</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>김콧치냥</t>
+          <t>현수기인</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>245</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2935,17 +2935,17 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2021년  2월 24일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
@@ -3016,17 +3016,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>흰색난닝구</t>
+          <t>스라맘</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>244</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>아크</t>
+          <t>엔젤릭버스터</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3036,29 +3036,29 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2020년  11월 22일</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>스라맘</t>
+          <t>흰색난닝구</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>245</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>엔젤릭버스터</t>
+          <t>아크</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3068,12 +3068,12 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2020년  11월 22일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
@@ -3144,64 +3144,64 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>뮤다양</t>
+          <t>왕눈이에깅</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>244</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>섀도어</t>
+          <t>소울마스터</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2021년  1월 31일</t>
+          <t>2019년  12월 22일</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>왕눈이에깅</t>
+          <t>뮤다양</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>245</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>소울마스터</t>
+          <t>섀도어</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2019년  12월 22일</t>
+          <t>2021년  1월 31일</t>
         </is>
       </c>
     </row>
@@ -3272,64 +3272,64 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>애르니로</t>
+          <t>반의반숙계란</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>244</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>윈드브레이커</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>반의반숙계란</t>
+          <t>애르니로</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>245</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>윈드브레이커</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
@@ -3368,17 +3368,17 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>소년선장</t>
+          <t>relize</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>244</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>캐논마스터</t>
+          <t>메르세데스</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3388,12 +3388,12 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2021년  1월 10일</t>
+          <t>2021년  1월 24일</t>
         </is>
       </c>
     </row>
@@ -3432,17 +3432,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>relize</t>
+          <t>소년선장</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>240</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>메르세데스</t>
+          <t>캐논마스터</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3452,12 +3452,12 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2021년  1월 24일</t>
+          <t>2021년  1월 10일</t>
         </is>
       </c>
     </row>
@@ -3496,32 +3496,32 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>RagSeIng</t>
+          <t>모범승기</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>호영</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2020년  5월 24일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
@@ -3560,49 +3560,49 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>모범승기</t>
+          <t>RagSeIng</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>240</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>호영</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2020년  5월 24일</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>쁘마유</t>
+          <t>유희왕이철민</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>235</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>소울마스터</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3617,39 +3617,39 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>유희왕이철민</t>
+          <t>띠르루</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>235</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>아크</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2021년  2월 24일</t>
         </is>
       </c>
     </row>
@@ -3688,32 +3688,32 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>띠르루</t>
+          <t>쁘마유</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>아크</t>
+          <t>소울마스터</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2021년  2월 24일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
@@ -3752,32 +3752,32 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>호돌너구리</t>
+          <t>암호엥</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>호영</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2020년  10월 4일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
@@ -3816,96 +3816,96 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>암호엥</t>
+          <t>호돌너구리</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>호영</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2020년  10월 4일</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>섀도구바</t>
+          <t>홍생강산초</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>235</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>섀도어</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2020년  12월 13일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>홍생강산초</t>
+          <t>홀윈브</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>235</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>윈드브레이커</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2020년  9월 20일</t>
         </is>
       </c>
     </row>
@@ -3944,32 +3944,32 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>홀윈브</t>
+          <t>섀도구바</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>윈드브레이커</t>
+          <t>섀도어</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2020년  9월 20일</t>
+          <t>2020년  12월 13일</t>
         </is>
       </c>
     </row>
@@ -4008,32 +4008,32 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>필승코찌</t>
+          <t>랄릎</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>캐논마스터</t>
+          <t>섀도어</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
@@ -4072,32 +4072,32 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>랄릎</t>
+          <t>필승코찌</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>섀도어</t>
+          <t>캐논마스터</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
@@ -4136,32 +4136,32 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>방구석빛쟁이</t>
+          <t>분홍은월해요</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>루미너스</t>
+          <t>은월</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2021년  1월 3일</t>
+          <t>2021년  1월 31일</t>
         </is>
       </c>
     </row>
@@ -4200,32 +4200,32 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>분홍은월해요</t>
+          <t>방구석빛쟁이</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>은월</t>
+          <t>루미너스</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2021년  1월 31일</t>
+          <t>2021년  1월 3일</t>
         </is>
       </c>
     </row>
@@ -4264,81 +4264,81 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>뽕짝스타</t>
+          <t>조뺘삐</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>엔젤릭버스터</t>
+          <t>나이트로드</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2020년  12월 27일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>망치엄마꺼</t>
+          <t>뽕짝스타</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>238</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>패스파인더</t>
+          <t>엔젤릭버스터</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2020년  12월 13일</t>
+          <t>2020년  12월 27일</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>조뺘삐</t>
+          <t>망치엄마꺼</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>나이트로드</t>
+          <t>패스파인더</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2020년  12월 13일</t>
         </is>
       </c>
     </row>
@@ -4392,64 +4392,64 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>tlfh</t>
+          <t>내섭그거</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>에반</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>내섭그거</t>
+          <t>tlfh</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>238</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>에반</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
@@ -4520,96 +4520,96 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>서울대맹구학</t>
+          <t>패파에폴트</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>스트라이커</t>
+          <t>패스파인더</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2020년  12월 27일</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>안휘가람</t>
+          <t>서울대맹구학</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>237</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>스트라이커</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>46</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>46</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>패파에폴트</t>
+          <t>안휘가람</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>232</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>패스파인더</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>2020년  12월 27일</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
@@ -4648,64 +4648,64 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>안래아</t>
+          <t>어줍</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>아크</t>
+          <t>에반</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2020년  7월 19일</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>어줍</t>
+          <t>안래아</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>237</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>에반</t>
+          <t>아크</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>2020년  7월 19일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
@@ -4776,96 +4776,96 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>아크아쿠마</t>
+          <t>represents</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>236</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>아크</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>43</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>2020년  9월 27일</t>
+          <t>2021년  2월 7일</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>세야낭</t>
+          <t>아크아쿠마</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>237</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>신궁</t>
+          <t>아크</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>2020년  10월 18일</t>
+          <t>2020년  9월 27일</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>represents</t>
+          <t>세야낭</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>231</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>신궁</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>44</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>2021년  2월 7일</t>
+          <t>2020년  10월 18일</t>
         </is>
       </c>
     </row>
@@ -4904,96 +4904,96 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>시비르</t>
+          <t>조선의박정수</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>235</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>은월</t>
+          <t>패스파인더</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>43</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>2021년  2월 14일</t>
+          <t>2020년  9월 27일</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>아스먕</t>
+          <t>시비르</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>237</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>비숍</t>
+          <t>은월</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>45</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2021년  2월 14일</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>조선의박정수</t>
+          <t>아스먕</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>235</t>
+          <t>231</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>패스파인더</t>
+          <t>비숍</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>2020년  9월 27일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
@@ -5064,12 +5064,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>잇긍</t>
+          <t>분홍분홍해영</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>228</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -5079,29 +5079,29 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>42</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>42</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>2020년  9월 6일</t>
+          <t>2021년  1월 31일</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>분홍분홍해영</t>
+          <t>잇긍</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>231</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -5111,17 +5111,17 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>43</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>2021년  1월 31일</t>
+          <t>2020년  9월 6일</t>
         </is>
       </c>
     </row>
@@ -5736,64 +5736,64 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>참새와병아리</t>
+          <t>셀리핥짝핥짝</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>225</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>비숍</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>기록없음</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>셀리핥짝핥짝</t>
+          <t>참새와병아리</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>221</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>비숍</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>기록없음</t>
         </is>
       </c>
     </row>
@@ -5992,64 +5992,64 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>뽀짜밍</t>
+          <t>플렉쭈</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>220</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>듀얼블레이더</t>
+          <t>아델</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>38</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>38</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>2020년  12월 13일</t>
+          <t>2020년  2월 9일</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>플렉쭈</t>
+          <t>뽀짜밍</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>230</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>아델</t>
+          <t>듀얼블레이더</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>37</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>29</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>2020년  2월 9일</t>
+          <t>2020년  12월 13일</t>
         </is>
       </c>
     </row>
@@ -6280,64 +6280,64 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>손야지</t>
+          <t>휴가다잉</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>229</t>
+          <t>220</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>배틀메이지</t>
+          <t>데몬어벤져</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>2021년  2월 21일</t>
+          <t>2019년  11월 3일</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>휴가다잉</t>
+          <t>손야지</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>229</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>데몬어벤져</t>
+          <t>배틀메이지</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>2019년  11월 3일</t>
+          <t>2021년  2월 21일</t>
         </is>
       </c>
     </row>

</xml_diff>